<commit_message>
Completed Arghman Book and 25 pages of Arooj-e-Iqbal
</commit_message>
<xml_diff>
--- a/instructions/Work record.xlsx
+++ b/instructions/Work record.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYP\BookReader\instructions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FINAL YEAR PROJECT\BookReader\instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85ED62B7-0E53-4E39-8C62-6527784EAB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA7B9CD-1CBE-4C76-A319-53264BEAAB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProgress" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Book Title</t>
   </si>
@@ -44,6 +44,27 @@
   </si>
   <si>
     <t>Ending Time of working</t>
+  </si>
+  <si>
+    <t>Armaghan-e-Hijaz (Urdu)</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>Arooj-e-Iqbal</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>22/09/2022</t>
+  </si>
+  <si>
+    <t>Resource Name</t>
+  </si>
+  <si>
+    <t>Azka Tariq</t>
   </si>
 </sst>
 </file>
@@ -84,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -305,48 +327,113 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="25.5546875" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>47</v>
+      </c>
+      <c r="F2">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 94 pages of Arroj-e-Iqbal by Azka
</commit_message>
<xml_diff>
--- a/instructions/Work record.xlsx
+++ b/instructions/Work record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FINAL YEAR PROJECT\BookReader\instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA7B9CD-1CBE-4C76-A319-53264BEAAB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D30FE45-A6AD-4CC7-B53D-5A7CEBFD12DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Book Title</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Azka Tariq</t>
+  </si>
+  <si>
+    <t>23/09/2022</t>
+  </si>
+  <si>
+    <t>1.5 hours</t>
   </si>
 </sst>
 </file>
@@ -327,10 +333,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -407,10 +413,13 @@
         <v>9</v>
       </c>
       <c r="J2">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -432,8 +441,37 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-      <c r="J3">
-        <v>25</v>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>119</v>
+      </c>
+      <c r="F4">
+        <v>94</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed 84 pages of Anjuman e Iqbal by Azka
</commit_message>
<xml_diff>
--- a/instructions/Work record.xlsx
+++ b/instructions/Work record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FINAL YEAR PROJECT\BookReader\instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D30FE45-A6AD-4CC7-B53D-5A7CEBFD12DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E37554-ECF5-4FBB-B21E-B476C02688B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Book Title</t>
   </si>
@@ -111,10 +111,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,10 +334,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -474,6 +475,32 @@
         <v>94</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>120</v>
+      </c>
+      <c r="E5">
+        <v>201</v>
+      </c>
+      <c r="F5">
+        <v>84</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>